<commit_message>
Fixed blank in identifier
</commit_message>
<xml_diff>
--- a/publication/v8.7/Peppol Code Lists - Document types v8.7.xlsx
+++ b/publication/v8.7/Peppol Code Lists - Document types v8.7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56ADEEA8-57DA-47CF-AFF4-B9CDDD742FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260EC26C-7435-4E25-932F-B07EE4ECC466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1217,28 +1217,13 @@
     <t>urn:oasis:names:specification:ubl:schema:xsd:TenderReceipt-2::TenderReceipt##urn:fdc:peppol.eu:prac:trns:t006:1.1::2.2</t>
   </si>
   <si>
-    <t xml:space="preserve">urn:oasis:names:specification:ubl:schema:xsd:Enquiry-2::Enquiry##urn:fdc:peppol.eu:prac:trns:t007:1.1::2.2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">urn:oasis:names:specification:ubl:schema:xsd:EnquiryResponse-2::EnquiryResponse##urn:fdc:peppol.eu:prac:trns:t008:1.1::2.2             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">urn:oasis:names:specification:ubl:schema:xsd:Enquiry-2::Enquiry##urn:fdc:peppol.eu:prac:trns:t009:1.1::2.2             </t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:EnquiryResponse-2::EnquiryResponse##urn:fdc:peppol.eu:prac:trns:t010:1.1::2.2</t>
   </si>
   <si>
-    <t xml:space="preserve">urn:oasis:names:tc:ebxml-regrep:xsd:query:4.0::QueryRequest##urn:fdc:peppol.eu:prac:trns:t011:1.1::4.0             </t>
-  </si>
-  <si>
     <t>urn:oasis:names:tc:ebxml-regrep:xsd:query:4.0::QueryResponse##urn:fdc:peppol.eu:prac:trns:t012:1.1::4.0</t>
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:TenderReceipt-2::TenderReceipt##urn:fdc:peppol.eu:prac:trns:t014:1.1::2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">urn:oasis:names:tc:ebxml-regrep:xsd:lcm:4.0::SubmitObjectsRequest##urn:fdc:peppol.eu:prac:trns:t015:1.1::4.0             </t>
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:fdc:peppol.eu:prac:trns:t016:1.1::2.2</t>
@@ -2039,12 +2024,6 @@
     <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:xeinkauf.de:kosit:xrechnung_3.0#conformant#urn:xeinkauf.de:kosit:extension:xrechnung_3.0::D16B</t>
   </si>
   <si>
-    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:xeinkauf.de:kosit:xrechnung_3.0#conformant#urn:xeinkauf. de:kosit:extension:xrechnung_3.0::2.1</t>
-  </si>
-  <si>
-    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:xeinkauf.de:kosit:xrechnung_3.0#conformant#urn:xeinkauf. de:kosit:extension:xrechnung_3.0::2.1</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:xeinkauf.de:kosit:xrechnung_3.0::2.1</t>
   </si>
   <si>
@@ -2067,6 +2046,27 @@
   </si>
   <si>
     <t>TICC-297</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:xeinkauf.de:kosit:xrechnung_3.0#conformant#urn:xeinkauf.de:kosit:extension:xrechnung_3.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Enquiry-2::Enquiry##urn:fdc:peppol.eu:prac:trns:t007:1.1::2.2</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:EnquiryResponse-2::EnquiryResponse##urn:fdc:peppol.eu:prac:trns:t008:1.1::2.2</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Enquiry-2::Enquiry##urn:fdc:peppol.eu:prac:trns:t009:1.1::2.2</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:tc:ebxml-regrep:xsd:query:4.0::QueryRequest##urn:fdc:peppol.eu:prac:trns:t011:1.1::4.0</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:tc:ebxml-regrep:xsd:lcm:4.0::SubmitObjectsRequest##urn:fdc:peppol.eu:prac:trns:t015:1.1::4.0</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:xeinkauf.de:kosit:xrechnung_3.0#conformant#urn:xeinkauf.de:kosit:extension:xrechnung_3.0::2.1</t>
   </si>
 </sst>
 </file>
@@ -2728,9 +2728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
   <dimension ref="A1:L245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K245" sqref="K245"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A225" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C246" sqref="C246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2761,22 +2761,22 @@
         <v>127</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="E1" s="23" t="s">
         <v>366</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>113</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="J1" s="23" t="s">
         <v>114</v>
@@ -3807,7 +3807,7 @@
     </row>
     <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>56</v>
@@ -3837,7 +3837,7 @@
     </row>
     <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>56</v>
@@ -3959,7 +3959,7 @@
     </row>
     <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>56</v>
@@ -3989,7 +3989,7 @@
     </row>
     <row r="38" spans="1:12" s="37" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="37" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="B38" s="32" t="s">
         <v>56</v>
@@ -4004,11 +4004,11 @@
         <v>367</v>
       </c>
       <c r="F38" s="39" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="G38" s="36"/>
       <c r="H38" s="37" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I38" s="37" t="b">
         <f>TRUE</f>
@@ -4026,7 +4026,7 @@
     </row>
     <row r="39" spans="1:12" s="37" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="37" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="B39" s="32" t="s">
         <v>56</v>
@@ -4041,11 +4041,11 @@
         <v>367</v>
       </c>
       <c r="F39" s="39" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="G39" s="36"/>
       <c r="H39" s="37" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I39" s="37" t="b">
         <f>TRUE</f>
@@ -4063,7 +4063,7 @@
     </row>
     <row r="40" spans="1:12" s="37" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="B40" s="32" t="s">
         <v>56</v>
@@ -4078,11 +4078,11 @@
         <v>367</v>
       </c>
       <c r="F40" s="39" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="G40" s="36"/>
       <c r="H40" s="37" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I40" s="37" t="b">
         <f>TRUE</f>
@@ -4100,7 +4100,7 @@
     </row>
     <row r="41" spans="1:12" s="37" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="37" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="B41" s="32" t="s">
         <v>56</v>
@@ -4115,11 +4115,11 @@
         <v>367</v>
       </c>
       <c r="F41" s="39" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="G41" s="36"/>
       <c r="H41" s="37" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I41" s="37" t="b">
         <f>TRUE</f>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="42" spans="1:12" s="37" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="B42" s="32" t="s">
         <v>56</v>
@@ -4152,11 +4152,11 @@
         <v>367</v>
       </c>
       <c r="F42" s="39" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="G42" s="36"/>
       <c r="H42" s="37" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I42" s="37" t="b">
         <f>TRUE</f>
@@ -4174,7 +4174,7 @@
     </row>
     <row r="43" spans="1:12" s="37" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="37" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="B43" s="32" t="s">
         <v>56</v>
@@ -4189,11 +4189,11 @@
         <v>367</v>
       </c>
       <c r="F43" s="39" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="G43" s="36"/>
       <c r="H43" s="37" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I43" s="37" t="b">
         <f>TRUE</f>
@@ -4223,7 +4223,7 @@
         <v>3</v>
       </c>
       <c r="E44" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F44" s="18">
         <v>5</v>
@@ -4232,7 +4232,7 @@
         <v>45070</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="I44" s="16" t="b">
         <f>FALSE</f>
@@ -4260,7 +4260,7 @@
         <v>3</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F45" s="18">
         <v>5</v>
@@ -4269,7 +4269,7 @@
         <v>45070</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="I45" s="16" t="b">
         <f>FALSE</f>
@@ -4297,7 +4297,7 @@
         <v>3</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F46" s="18">
         <v>5</v>
@@ -4306,7 +4306,7 @@
         <v>45070</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="I46" s="16" t="b">
         <f>FALSE</f>
@@ -4337,7 +4337,7 @@
         <v>368</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="I47" s="5" t="b">
         <f>FALSE</f>
@@ -4367,7 +4367,7 @@
         <v>368</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="I48" s="5" t="b">
         <f>FALSE</f>
@@ -4397,7 +4397,7 @@
         <v>368</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I49" s="5" t="b">
         <f>FALSE</f>
@@ -4427,7 +4427,7 @@
         <v>368</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I50" s="5" t="b">
         <f>FALSE</f>
@@ -4442,7 +4442,7 @@
     </row>
     <row r="51" spans="1:12" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="37" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="B51" s="32" t="s">
         <v>56</v>
@@ -4476,7 +4476,7 @@
     </row>
     <row r="52" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>56</v>
@@ -4506,7 +4506,7 @@
     </row>
     <row r="53" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>56</v>
@@ -4536,7 +4536,7 @@
     </row>
     <row r="54" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>56</v>
@@ -4551,7 +4551,7 @@
         <v>368</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="I54" s="5" t="b">
         <f>TRUE</f>
@@ -4564,12 +4564,12 @@
         <v>117</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>56</v>
@@ -4599,7 +4599,7 @@
     </row>
     <row r="56" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>56</v>
@@ -4629,7 +4629,7 @@
     </row>
     <row r="57" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>56</v>
@@ -4659,7 +4659,7 @@
     </row>
     <row r="58" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>56</v>
@@ -4689,7 +4689,7 @@
     </row>
     <row r="59" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>56</v>
@@ -4719,7 +4719,7 @@
     </row>
     <row r="60" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>56</v>
@@ -4803,7 +4803,7 @@
     </row>
     <row r="63" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>56</v>
@@ -4852,7 +4852,7 @@
       </c>
       <c r="G64" s="36"/>
       <c r="H64" s="37" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="I64" s="37" t="b">
         <f>TRUE</f>
@@ -4870,7 +4870,7 @@
     </row>
     <row r="65" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>56</v>
@@ -4885,7 +4885,7 @@
         <v>368</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="I65" s="5" t="b">
         <f>TRUE</f>
@@ -4915,16 +4915,16 @@
         <v>5</v>
       </c>
       <c r="E66" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F66" s="21" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="G66" s="19">
         <v>45070</v>
       </c>
       <c r="H66" s="16" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="I66" s="16" t="b">
         <f>FALSE</f>
@@ -4952,16 +4952,16 @@
         <v>5</v>
       </c>
       <c r="E67" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F67" s="21" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="G67" s="19">
         <v>45070</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="I67" s="16" t="b">
         <f>FALSE</f>
@@ -4989,16 +4989,16 @@
         <v>5</v>
       </c>
       <c r="E68" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F68" s="21" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="G68" s="19">
         <v>45070</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="I68" s="16" t="b">
         <f>FALSE</f>
@@ -5104,7 +5104,7 @@
     </row>
     <row r="72" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>56</v>
@@ -5137,7 +5137,7 @@
     </row>
     <row r="73" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>56</v>
@@ -5242,16 +5242,16 @@
         <v>6</v>
       </c>
       <c r="E76" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F76" s="21" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="G76" s="19">
         <v>45292</v>
       </c>
       <c r="H76" s="16" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="I76" s="16" t="b">
         <f>FALSE</f>
@@ -5279,16 +5279,16 @@
         <v>6</v>
       </c>
       <c r="E77" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F77" s="21" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="G77" s="19">
         <v>45292</v>
       </c>
       <c r="H77" s="16" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="I77" s="16" t="b">
         <f>FALSE</f>
@@ -5316,7 +5316,7 @@
         <v>7</v>
       </c>
       <c r="E78" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F78" s="21" t="s">
         <v>206</v>
@@ -5325,7 +5325,7 @@
         <v>45070</v>
       </c>
       <c r="H78" s="16" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="I78" s="16" t="b">
         <f>FALSE</f>
@@ -5353,7 +5353,7 @@
         <v>7</v>
       </c>
       <c r="E79" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F79" s="21" t="s">
         <v>206</v>
@@ -5362,7 +5362,7 @@
         <v>45070</v>
       </c>
       <c r="H79" s="16" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="I79" s="16" t="b">
         <f>FALSE</f>
@@ -5390,7 +5390,7 @@
         <v>7</v>
       </c>
       <c r="E80" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F80" s="21" t="s">
         <v>206</v>
@@ -5399,7 +5399,7 @@
         <v>45070</v>
       </c>
       <c r="H80" s="16" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="I80" s="16" t="b">
         <f>FALSE</f>
@@ -5487,7 +5487,7 @@
         <v>7</v>
       </c>
       <c r="E83" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F83" s="22" t="s">
         <v>244</v>
@@ -5496,7 +5496,7 @@
         <v>45070</v>
       </c>
       <c r="H83" s="16" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="I83" s="16" t="b">
         <f>FALSE</f>
@@ -5554,7 +5554,7 @@
         <v>7</v>
       </c>
       <c r="E85" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F85" s="21" t="s">
         <v>206</v>
@@ -5563,7 +5563,7 @@
         <v>45070</v>
       </c>
       <c r="H85" s="16" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="I85" s="16" t="b">
         <f>FALSE</f>
@@ -5591,7 +5591,7 @@
         <v>7</v>
       </c>
       <c r="E86" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F86" s="21" t="s">
         <v>206</v>
@@ -5600,7 +5600,7 @@
         <v>45070</v>
       </c>
       <c r="H86" s="16" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="I86" s="16" t="b">
         <f>FALSE</f>
@@ -5628,7 +5628,7 @@
         <v>7</v>
       </c>
       <c r="E87" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F87" s="21" t="s">
         <v>206</v>
@@ -5637,7 +5637,7 @@
         <v>45070</v>
       </c>
       <c r="H87" s="16" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="I87" s="16" t="b">
         <f>FALSE</f>
@@ -5985,7 +5985,7 @@
         <v>206</v>
       </c>
       <c r="E98" s="25" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F98" s="22" t="s">
         <v>244</v>
@@ -5994,7 +5994,7 @@
         <v>45070</v>
       </c>
       <c r="H98" s="16" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="I98" s="16" t="b">
         <f>FALSE</f>
@@ -6182,7 +6182,7 @@
         <v>117</v>
       </c>
       <c r="L104" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="105" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -6272,7 +6272,7 @@
         <v>117</v>
       </c>
       <c r="L107" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="108" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -6302,7 +6302,7 @@
         <v>365</v>
       </c>
       <c r="L108" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="109" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -6332,7 +6332,7 @@
         <v>365</v>
       </c>
       <c r="L109" s="5" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="110" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -6362,7 +6362,7 @@
         <v>365</v>
       </c>
       <c r="L110" s="5" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -6392,7 +6392,7 @@
         <v>365</v>
       </c>
       <c r="L111" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="112" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -6422,7 +6422,7 @@
         <v>365</v>
       </c>
       <c r="L112" s="5" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="113" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -6452,7 +6452,7 @@
         <v>365</v>
       </c>
       <c r="L113" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="114" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -6482,7 +6482,7 @@
         <v>365</v>
       </c>
       <c r="L114" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="115" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -6512,7 +6512,7 @@
         <v>365</v>
       </c>
       <c r="L115" s="5" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="116" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -6542,7 +6542,7 @@
         <v>365</v>
       </c>
       <c r="L116" s="5" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="117" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -6572,7 +6572,7 @@
         <v>365</v>
       </c>
       <c r="L117" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="118" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -6602,7 +6602,7 @@
         <v>365</v>
       </c>
       <c r="L118" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="119" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -6632,7 +6632,7 @@
         <v>365</v>
       </c>
       <c r="L119" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="120" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -6662,7 +6662,7 @@
         <v>365</v>
       </c>
       <c r="L120" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="121" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -6692,7 +6692,7 @@
         <v>365</v>
       </c>
       <c r="L121" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="122" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -6722,7 +6722,7 @@
         <v>365</v>
       </c>
       <c r="L122" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="123" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -6937,13 +6937,13 @@
     </row>
     <row r="130" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D130" s="29" t="s">
         <v>296</v>
@@ -6969,7 +6969,7 @@
     </row>
     <row r="131" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="B131" s="5" t="s">
         <v>56</v>
@@ -7001,13 +7001,13 @@
     </row>
     <row r="132" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="D132" s="29" t="s">
         <v>296</v>
@@ -7033,7 +7033,7 @@
     </row>
     <row r="133" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>56</v>
@@ -7732,7 +7732,7 @@
     </row>
     <row r="157" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="B157" s="4" t="s">
         <v>56</v>
@@ -7747,7 +7747,7 @@
         <v>368</v>
       </c>
       <c r="H157" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I157" s="5" t="b">
         <v>1</v>
@@ -7759,12 +7759,12 @@
         <v>116</v>
       </c>
       <c r="L157" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="158" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="B158" s="4" t="s">
         <v>56</v>
@@ -7779,7 +7779,7 @@
         <v>368</v>
       </c>
       <c r="H158" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I158" s="5" t="b">
         <v>1</v>
@@ -7791,12 +7791,12 @@
         <v>116</v>
       </c>
       <c r="L158" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="159" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B159" s="4" t="s">
         <v>56</v>
@@ -7811,7 +7811,7 @@
         <v>368</v>
       </c>
       <c r="H159" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I159" s="5" t="b">
         <v>1</v>
@@ -7823,12 +7823,12 @@
         <v>116</v>
       </c>
       <c r="L159" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="160" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="B160" s="4" t="s">
         <v>56</v>
@@ -7843,7 +7843,7 @@
         <v>368</v>
       </c>
       <c r="H160" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I160" s="5" t="b">
         <v>1</v>
@@ -7855,12 +7855,12 @@
         <v>116</v>
       </c>
       <c r="L160" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B161" s="4" t="s">
         <v>56</v>
@@ -7875,7 +7875,7 @@
         <v>368</v>
       </c>
       <c r="H161" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I161" s="5" t="b">
         <v>1</v>
@@ -7887,12 +7887,12 @@
         <v>116</v>
       </c>
       <c r="L161" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="162" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B162" s="4" t="s">
         <v>56</v>
@@ -7907,7 +7907,7 @@
         <v>368</v>
       </c>
       <c r="H162" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I162" s="5" t="b">
         <v>1</v>
@@ -7919,18 +7919,18 @@
         <v>116</v>
       </c>
       <c r="L162" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="163" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="B163" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>385</v>
+        <v>654</v>
       </c>
       <c r="D163" s="29" t="s">
         <v>296</v>
@@ -7939,7 +7939,7 @@
         <v>368</v>
       </c>
       <c r="H163" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I163" s="5" t="b">
         <v>1</v>
@@ -7951,18 +7951,18 @@
         <v>116</v>
       </c>
       <c r="L163" s="5" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="164" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B164" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>386</v>
+        <v>655</v>
       </c>
       <c r="D164" s="29" t="s">
         <v>296</v>
@@ -7971,7 +7971,7 @@
         <v>368</v>
       </c>
       <c r="H164" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I164" s="5" t="b">
         <v>1</v>
@@ -7983,18 +7983,18 @@
         <v>116</v>
       </c>
       <c r="L164" s="5" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="165" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="B165" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>387</v>
+        <v>656</v>
       </c>
       <c r="D165" s="29" t="s">
         <v>296</v>
@@ -8003,7 +8003,7 @@
         <v>368</v>
       </c>
       <c r="H165" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I165" s="5" t="b">
         <v>1</v>
@@ -8015,18 +8015,18 @@
         <v>116</v>
       </c>
       <c r="L165" s="5" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="166" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B166" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D166" s="29" t="s">
         <v>296</v>
@@ -8035,7 +8035,7 @@
         <v>368</v>
       </c>
       <c r="H166" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I166" s="5" t="b">
         <v>1</v>
@@ -8047,18 +8047,18 @@
         <v>116</v>
       </c>
       <c r="L166" s="5" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="B167" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>389</v>
+        <v>657</v>
       </c>
       <c r="D167" s="29" t="s">
         <v>296</v>
@@ -8067,7 +8067,7 @@
         <v>368</v>
       </c>
       <c r="H167" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I167" s="5" t="b">
         <v>1</v>
@@ -8079,18 +8079,18 @@
         <v>116</v>
       </c>
       <c r="L167" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="168" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B168" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D168" s="29" t="s">
         <v>296</v>
@@ -8099,7 +8099,7 @@
         <v>368</v>
       </c>
       <c r="H168" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I168" s="5" t="b">
         <v>1</v>
@@ -8111,18 +8111,18 @@
         <v>116</v>
       </c>
       <c r="L168" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="169" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B169" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="D169" s="29" t="s">
         <v>296</v>
@@ -8131,7 +8131,7 @@
         <v>368</v>
       </c>
       <c r="H169" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I169" s="5" t="b">
         <v>1</v>
@@ -8143,18 +8143,18 @@
         <v>116</v>
       </c>
       <c r="L169" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="170" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B170" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D170" s="29" t="s">
         <v>296</v>
@@ -8163,7 +8163,7 @@
         <v>368</v>
       </c>
       <c r="H170" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I170" s="5" t="b">
         <v>1</v>
@@ -8175,18 +8175,18 @@
         <v>116</v>
       </c>
       <c r="L170" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="171" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="B171" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>392</v>
+        <v>658</v>
       </c>
       <c r="D171" s="29" t="s">
         <v>296</v>
@@ -8195,7 +8195,7 @@
         <v>368</v>
       </c>
       <c r="H171" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I171" s="5" t="b">
         <v>1</v>
@@ -8207,18 +8207,18 @@
         <v>116</v>
       </c>
       <c r="L171" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="172" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="B172" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D172" s="29" t="s">
         <v>296</v>
@@ -8227,7 +8227,7 @@
         <v>368</v>
       </c>
       <c r="H172" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="I172" s="5" t="b">
         <v>1</v>
@@ -8239,18 +8239,18 @@
         <v>116</v>
       </c>
       <c r="L172" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="173" spans="1:12" s="37" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A173" s="37" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="B173" s="32" t="s">
         <v>56</v>
       </c>
       <c r="C173" s="37" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="D173" s="38" t="s">
         <v>296</v>
@@ -8259,11 +8259,11 @@
         <v>367</v>
       </c>
       <c r="F173" s="39" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="G173" s="36"/>
       <c r="H173" s="37" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="I173" s="37" t="b">
         <v>1</v>
@@ -8275,27 +8275,27 @@
         <v>116</v>
       </c>
       <c r="L173" s="37" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="174" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B174" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="D174" s="29" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E174" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H174" s="5" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="I174" s="5" t="b">
         <v>1</v>
@@ -8307,27 +8307,27 @@
         <v>116</v>
       </c>
       <c r="L174" s="5" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="175" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="B175" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D175" s="29" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="E175" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H175" s="5" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="I175" s="5" t="b">
         <v>0</v>
@@ -8341,22 +8341,22 @@
     </row>
     <row r="176" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C176" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="D176" s="29" t="s">
         <v>434</v>
       </c>
-      <c r="B176" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C176" s="5" t="s">
+      <c r="E176" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H176" s="5" t="s">
         <v>441</v>
-      </c>
-      <c r="D176" s="29" t="s">
-        <v>439</v>
-      </c>
-      <c r="E176" s="24" t="s">
-        <v>368</v>
-      </c>
-      <c r="H176" s="5" t="s">
-        <v>446</v>
       </c>
       <c r="I176" s="5" t="b">
         <v>0</v>
@@ -8370,22 +8370,22 @@
     </row>
     <row r="177" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B177" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="D177" s="29" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="E177" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H177" s="5" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="I177" s="5" t="b">
         <v>0</v>
@@ -8399,22 +8399,22 @@
     </row>
     <row r="178" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="B178" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D178" s="29" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="E178" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H178" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I178" s="5" t="b">
         <v>0</v>
@@ -8428,22 +8428,22 @@
     </row>
     <row r="179" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B179" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="D179" s="29" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="E179" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H179" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I179" s="5" t="b">
         <v>0</v>
@@ -8457,22 +8457,22 @@
     </row>
     <row r="180" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="B180" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="D180" s="29" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="E180" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H180" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I180" s="5" t="b">
         <v>0</v>
@@ -8486,90 +8486,90 @@
     </row>
     <row r="181" spans="1:12" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="37" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="B181" s="32" t="s">
         <v>56</v>
       </c>
       <c r="C181" s="37" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D181" s="38" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="E181" s="34" t="s">
         <v>367</v>
       </c>
       <c r="F181" s="41" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="G181" s="36"/>
       <c r="H181" s="37" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="I181" s="37" t="b">
         <v>1</v>
       </c>
       <c r="J181" s="34"/>
       <c r="K181" s="34" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="L181" s="37" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="182" spans="1:12" s="37" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" s="37" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="B182" s="32" t="s">
         <v>56</v>
       </c>
       <c r="C182" s="37" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="D182" s="38" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="E182" s="34" t="s">
         <v>367</v>
       </c>
       <c r="F182" s="41" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="G182" s="36"/>
       <c r="H182" s="37" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="I182" s="37" t="b">
         <v>1</v>
       </c>
       <c r="J182" s="34"/>
       <c r="K182" s="34" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="L182" s="37" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="183" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="B183" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="D183" s="29" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="E183" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H183" s="5" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="I183" s="5" t="b">
         <v>1</v>
@@ -8578,30 +8578,30 @@
         <v>1</v>
       </c>
       <c r="K183" s="24" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="L183" s="15" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="184" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="B184" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="D184" s="29" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="E184" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H184" s="5" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="I184" s="5" t="b">
         <v>1</v>
@@ -8610,30 +8610,30 @@
         <v>1</v>
       </c>
       <c r="K184" s="24" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="L184" s="14" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="185" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="B185" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="D185" s="29" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="E185" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H185" s="5" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="I185" s="5" t="b">
         <v>1</v>
@@ -8642,30 +8642,30 @@
         <v>1</v>
       </c>
       <c r="K185" s="24" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="L185" s="14" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="186" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B186" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="D186" s="28" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="E186" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H186" s="5" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="I186" s="5" t="b">
         <v>0</v>
@@ -8674,27 +8674,27 @@
         <v>117</v>
       </c>
       <c r="L186" s="5" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="187" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="B187" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="D187" s="28" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="E187" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H187" s="5" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="I187" s="5" t="b">
         <v>0</v>
@@ -8708,22 +8708,22 @@
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="B188" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D188" s="28" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="E188" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H188" s="5" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="I188" s="5" t="b">
         <f>TRUE</f>
@@ -8741,22 +8741,22 @@
     </row>
     <row r="189" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="B189" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C189" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="D189" s="28" t="s">
         <v>500</v>
       </c>
-      <c r="D189" s="28" t="s">
-        <v>505</v>
-      </c>
       <c r="E189" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H189" s="5" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="I189" s="5" t="b">
         <v>1</v>
@@ -8768,27 +8768,27 @@
         <v>117</v>
       </c>
       <c r="L189" s="5" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
     </row>
     <row r="190" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="B190" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="D190" s="28" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="E190" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H190" s="5" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="I190" s="5" t="b">
         <v>1</v>
@@ -8800,27 +8800,27 @@
         <v>117</v>
       </c>
       <c r="L190" s="5" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
     </row>
     <row r="191" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B191" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="D191" s="28" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="E191" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H191" s="5" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="I191" s="5" t="b">
         <v>1</v>
@@ -8832,27 +8832,27 @@
         <v>117</v>
       </c>
       <c r="L191" s="5" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
     </row>
     <row r="192" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="B192" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D192" s="29" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="E192" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H192" s="5" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="I192" s="5" t="b">
         <v>0</v>
@@ -8866,22 +8866,22 @@
     </row>
     <row r="193" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="B193" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C193" s="5" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="D193" s="29" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="E193" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H193" s="5" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="I193" s="5" t="b">
         <v>0</v>
@@ -8895,22 +8895,22 @@
     </row>
     <row r="194" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="B194" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C194" s="5" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="D194" s="29" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="E194" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H194" s="5" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="I194" s="5" t="b">
         <v>0</v>
@@ -8924,22 +8924,22 @@
     </row>
     <row r="195" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C195" s="5" t="s">
         <v>525</v>
       </c>
-      <c r="B195" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C195" s="5" t="s">
-        <v>530</v>
-      </c>
       <c r="D195" s="29" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="E195" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H195" s="5" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="I195" s="5" t="b">
         <v>0</v>
@@ -8953,22 +8953,22 @@
     </row>
     <row r="196" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C196" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="D196" s="29" t="s">
+        <v>515</v>
+      </c>
+      <c r="E196" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H196" s="5" t="s">
         <v>526</v>
-      </c>
-      <c r="B196" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C196" s="5" t="s">
-        <v>528</v>
-      </c>
-      <c r="D196" s="29" t="s">
-        <v>520</v>
-      </c>
-      <c r="E196" s="24" t="s">
-        <v>368</v>
-      </c>
-      <c r="H196" s="5" t="s">
-        <v>531</v>
       </c>
       <c r="I196" s="5" t="b">
         <v>0</v>
@@ -8982,22 +8982,22 @@
     </row>
     <row r="197" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="B197" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C197" s="5" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="D197" s="29" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="E197" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H197" s="5" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="I197" s="5" t="b">
         <v>0</v>
@@ -9011,22 +9011,22 @@
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="B198" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="D198" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E198" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H198" s="5" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="I198" s="5" t="b">
         <f>TRUE</f>
@@ -9039,27 +9039,27 @@
         <v>117</v>
       </c>
       <c r="L198" s="7" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="199" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="B199" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C199" s="5" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="D199" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E199" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H199" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I199" s="5" t="b">
         <f>TRUE</f>
@@ -9072,27 +9072,27 @@
         <v>116</v>
       </c>
       <c r="L199" s="5" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
     </row>
     <row r="200" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="B200" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C200" s="5" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="D200" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E200" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H200" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I200" s="5" t="b">
         <f>TRUE</f>
@@ -9105,27 +9105,27 @@
         <v>116</v>
       </c>
       <c r="L200" s="5" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
     </row>
     <row r="201" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="B201" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C201" s="5" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D201" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E201" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H201" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I201" s="5" t="b">
         <f>TRUE</f>
@@ -9138,27 +9138,27 @@
         <v>116</v>
       </c>
       <c r="L201" s="5" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
     </row>
     <row r="202" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="B202" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C202" s="5" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="D202" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E202" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H202" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I202" s="5" t="b">
         <f>TRUE</f>
@@ -9171,27 +9171,27 @@
         <v>116</v>
       </c>
       <c r="L202" s="5" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
     </row>
     <row r="203" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="B203" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C203" s="5" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="D203" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E203" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H203" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I203" s="5" t="b">
         <v>1</v>
@@ -9203,27 +9203,27 @@
         <v>116</v>
       </c>
       <c r="L203" s="5" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
     </row>
     <row r="204" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="B204" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C204" s="5" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="D204" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E204" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H204" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I204" s="5" t="b">
         <v>1</v>
@@ -9235,27 +9235,27 @@
         <v>116</v>
       </c>
       <c r="L204" s="5" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="B205" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C205" s="5" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="D205" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E205" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H205" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I205" s="5" t="b">
         <v>1</v>
@@ -9267,27 +9267,27 @@
         <v>116</v>
       </c>
       <c r="L205" s="5" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="206" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="B206" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C206" s="5" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="D206" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E206" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H206" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I206" s="5" t="b">
         <v>1</v>
@@ -9299,27 +9299,27 @@
         <v>116</v>
       </c>
       <c r="L206" s="5" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="B207" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C207" s="5" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="D207" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E207" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H207" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I207" s="5" t="b">
         <v>1</v>
@@ -9331,27 +9331,27 @@
         <v>116</v>
       </c>
       <c r="L207" s="5" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
     </row>
     <row r="208" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="B208" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C208" s="5" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="D208" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E208" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H208" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I208" s="5" t="b">
         <v>1</v>
@@ -9363,27 +9363,27 @@
         <v>116</v>
       </c>
       <c r="L208" s="5" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
     </row>
     <row r="209" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="B209" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C209" s="5" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="D209" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E209" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H209" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I209" s="5" t="b">
         <v>1</v>
@@ -9395,27 +9395,27 @@
         <v>116</v>
       </c>
       <c r="L209" s="5" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
     </row>
     <row r="210" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="B210" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C210" s="5" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="D210" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E210" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H210" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I210" s="5" t="b">
         <v>1</v>
@@ -9427,27 +9427,27 @@
         <v>116</v>
       </c>
       <c r="L210" s="5" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
     </row>
     <row r="211" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="B211" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C211" s="5" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="D211" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E211" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H211" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I211" s="5" t="b">
         <v>1</v>
@@ -9459,27 +9459,27 @@
         <v>116</v>
       </c>
       <c r="L211" s="5" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
     </row>
     <row r="212" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="B212" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C212" s="5" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="D212" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E212" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H212" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I212" s="5" t="b">
         <v>1</v>
@@ -9491,27 +9491,27 @@
         <v>116</v>
       </c>
       <c r="L212" s="5" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
     </row>
     <row r="213" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="B213" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C213" s="5" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="D213" s="28" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E213" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H213" s="5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I213" s="5" t="b">
         <v>1</v>
@@ -9523,27 +9523,27 @@
         <v>116</v>
       </c>
       <c r="L213" s="5" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
     </row>
     <row r="214" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="B214" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C214" s="5" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="D214" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E214" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H214" s="5" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="I214" s="5" t="b">
         <v>1</v>
@@ -9552,30 +9552,30 @@
         <v>1</v>
       </c>
       <c r="K214" s="24" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="L214" s="43" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="215" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="B215" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C215" s="5" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="D215" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E215" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H215" s="5" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="I215" s="5" t="b">
         <v>1</v>
@@ -9584,30 +9584,30 @@
         <v>1</v>
       </c>
       <c r="K215" s="24" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="L215" s="43" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
     </row>
     <row r="216" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="B216" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C216" s="5" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="D216" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E216" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H216" s="5" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="I216" s="5" t="b">
         <v>1</v>
@@ -9616,30 +9616,30 @@
         <v>1</v>
       </c>
       <c r="K216" s="24" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="L216" s="43" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
     </row>
     <row r="217" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="B217" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C217" s="5" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="D217" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E217" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H217" s="5" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="I217" s="5" t="b">
         <v>1</v>
@@ -9648,30 +9648,30 @@
         <v>1</v>
       </c>
       <c r="K217" s="24" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="L217" s="43" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
     </row>
     <row r="218" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="B218" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C218" s="5" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="D218" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E218" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H218" s="5" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="I218" s="5" t="b">
         <v>1</v>
@@ -9680,30 +9680,30 @@
         <v>1</v>
       </c>
       <c r="K218" s="24" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="L218" s="43" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
     </row>
     <row r="219" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="B219" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C219" s="5" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="D219" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E219" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H219" s="5" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="I219" s="5" t="b">
         <v>1</v>
@@ -9712,117 +9712,117 @@
         <v>1</v>
       </c>
       <c r="K219" s="24" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="L219" s="43" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="B220" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C220" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="D220" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E220" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H220" s="5" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="I220" s="5" t="b">
         <v>0</v>
       </c>
       <c r="K220" s="24" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="L220" s="5" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
     <row r="221" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="B221" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C221" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="D221" s="28" t="s">
+        <v>595</v>
+      </c>
+      <c r="E221" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H221" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="I221" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K221" s="24" t="s">
+        <v>445</v>
+      </c>
+      <c r="L221" s="5" t="s">
         <v>612</v>
-      </c>
-      <c r="B221" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C221" s="5" t="s">
-        <v>615</v>
-      </c>
-      <c r="D221" s="28" t="s">
-        <v>600</v>
-      </c>
-      <c r="E221" s="24" t="s">
-        <v>368</v>
-      </c>
-      <c r="H221" s="5" t="s">
-        <v>614</v>
-      </c>
-      <c r="I221" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K221" s="24" t="s">
-        <v>450</v>
-      </c>
-      <c r="L221" s="5" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="222" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="B222" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C222" s="5" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="D222" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E222" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H222" s="5" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="I222" s="5" t="b">
         <v>1</v>
       </c>
       <c r="K222" s="24" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="L222" s="5" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="C223" s="5" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="D223" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E223" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H223" s="5" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="I223" s="5" t="b">
         <v>1</v>
@@ -9834,27 +9834,27 @@
         <v>117</v>
       </c>
       <c r="L223" s="5" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="C224" s="5" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="D224" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E224" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H224" s="5" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="I224" s="5" t="b">
         <v>1</v>
@@ -9866,27 +9866,27 @@
         <v>117</v>
       </c>
       <c r="L224" s="5" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="B225" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C225" s="5" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="D225" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E225" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H225" s="5" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="I225" s="5" t="b">
         <v>1</v>
@@ -9898,27 +9898,27 @@
         <v>117</v>
       </c>
       <c r="L225" s="5" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="C226" s="5" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="D226" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E226" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H226" s="5" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="I226" s="5" t="b">
         <v>1</v>
@@ -9930,27 +9930,27 @@
         <v>117</v>
       </c>
       <c r="L226" s="5" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="C227" s="5" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="D227" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E227" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H227" s="5" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="I227" s="5" t="b">
         <v>0</v>
@@ -9962,27 +9962,27 @@
         <v>117</v>
       </c>
       <c r="L227" s="5" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="228" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="B228" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C228" s="5" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="D228" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E228" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H228" s="5" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="I228" s="5" t="b">
         <v>0</v>
@@ -9994,27 +9994,27 @@
         <v>117</v>
       </c>
       <c r="L228" s="5" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="229" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="C229" s="5" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="D229" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E229" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H229" s="5" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="I229" s="5" t="b">
         <v>0</v>
@@ -10026,27 +10026,27 @@
         <v>117</v>
       </c>
       <c r="L229" s="5" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230" s="5" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="B230" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C230" s="5" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="D230" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E230" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H230" s="5" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="I230" s="5" t="b">
         <v>1</v>
@@ -10058,27 +10058,27 @@
         <v>117</v>
       </c>
       <c r="L230" s="5" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="231" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" s="5" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="B231" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C231" s="5" t="s">
+        <v>628</v>
+      </c>
+      <c r="D231" s="28" t="s">
+        <v>595</v>
+      </c>
+      <c r="E231" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H231" s="5" t="s">
         <v>633</v>
-      </c>
-      <c r="D231" s="28" t="s">
-        <v>600</v>
-      </c>
-      <c r="E231" s="24" t="s">
-        <v>368</v>
-      </c>
-      <c r="H231" s="5" t="s">
-        <v>638</v>
       </c>
       <c r="I231" s="5" t="b">
         <v>1</v>
@@ -10090,27 +10090,27 @@
         <v>117</v>
       </c>
       <c r="L231" s="5" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="232" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="B232" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="D232" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E232" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H232" s="5" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="I232" s="5" t="b">
         <v>0</v>
@@ -10122,27 +10122,27 @@
         <v>117</v>
       </c>
       <c r="L232" s="5" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="233" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="B233" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C233" s="5" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="D233" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E233" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H233" s="5" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="I233" s="5" t="b">
         <v>0</v>
@@ -10154,27 +10154,27 @@
         <v>117</v>
       </c>
       <c r="L233" s="5" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234" s="5" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="C234" s="5" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="D234" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E234" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H234" s="5" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="I234" s="5" t="b">
         <v>1</v>
@@ -10186,27 +10186,27 @@
         <v>117</v>
       </c>
       <c r="L234" s="5" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="235" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A235" s="5" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="C235" s="5" t="s">
+        <v>628</v>
+      </c>
+      <c r="D235" s="28" t="s">
+        <v>595</v>
+      </c>
+      <c r="E235" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H235" s="5" t="s">
         <v>633</v>
-      </c>
-      <c r="D235" s="28" t="s">
-        <v>600</v>
-      </c>
-      <c r="E235" s="24" t="s">
-        <v>368</v>
-      </c>
-      <c r="H235" s="5" t="s">
-        <v>638</v>
       </c>
       <c r="I235" s="5" t="b">
         <v>1</v>
@@ -10218,27 +10218,27 @@
         <v>117</v>
       </c>
       <c r="L235" s="5" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="236" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A236" s="5" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="C236" s="5" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="D236" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E236" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H236" s="5" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="I236" s="5" t="b">
         <v>0</v>
@@ -10250,27 +10250,27 @@
         <v>117</v>
       </c>
       <c r="L236" s="5" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="237" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A237" s="5" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="C237" s="5" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="D237" s="28" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E237" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H237" s="5" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="I237" s="5" t="b">
         <v>0</v>
@@ -10282,27 +10282,27 @@
         <v>117</v>
       </c>
       <c r="L237" s="5" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="238" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="5" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="B238" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C238" s="5" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="D238" s="29" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="E238" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H238" s="5" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="I238" s="5" t="b">
         <v>0</v>
@@ -10316,22 +10316,22 @@
     </row>
     <row r="239" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A239" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C239" s="5" t="s">
+        <v>646</v>
+      </c>
+      <c r="D239" s="29" t="s">
+        <v>634</v>
+      </c>
+      <c r="E239" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H239" s="5" t="s">
         <v>642</v>
-      </c>
-      <c r="B239" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C239" s="5" t="s">
-        <v>653</v>
-      </c>
-      <c r="D239" s="29" t="s">
-        <v>639</v>
-      </c>
-      <c r="E239" s="24" t="s">
-        <v>368</v>
-      </c>
-      <c r="H239" s="5" t="s">
-        <v>647</v>
       </c>
       <c r="I239" s="5" t="b">
         <v>0</v>
@@ -10345,22 +10345,22 @@
     </row>
     <row r="240" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="B240" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C240" s="5" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="D240" s="29" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="E240" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H240" s="5" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="I240" s="5" t="b">
         <v>0</v>
@@ -10374,22 +10374,22 @@
     </row>
     <row r="241" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A241" s="5" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="B241" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C241" s="5" t="s">
-        <v>651</v>
+        <v>659</v>
       </c>
       <c r="D241" s="29" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="E241" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H241" s="5" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="I241" s="5" t="b">
         <v>0</v>
@@ -10403,22 +10403,22 @@
     </row>
     <row r="242" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A242" s="5" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="B242" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C242" s="5" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="D242" s="29" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="E242" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H242" s="5" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="I242" s="5" t="b">
         <v>0</v>
@@ -10432,22 +10432,22 @@
     </row>
     <row r="243" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A243" s="5" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="B243" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C243" s="5" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="D243" s="29" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="E243" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H243" s="5" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="I243" s="5" t="b">
         <v>0</v>
@@ -10461,22 +10461,22 @@
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" s="5" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="B244" s="5" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="C244" s="5" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="D244" s="29" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="E244" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H244" s="5" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="I244" s="5" t="b">
         <v>1</v>
@@ -10488,27 +10488,27 @@
         <v>117</v>
       </c>
       <c r="L244" s="5" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="245" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A245" s="5" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="C245" s="5" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="D245" s="29" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="E245" s="24" t="s">
         <v>368</v>
       </c>
       <c r="H245" s="5" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="I245" s="5" t="b">
         <v>1</v>
@@ -10520,7 +10520,7 @@
         <v>117</v>
       </c>
       <c r="L245" s="5" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>